<commit_message>
Tech deb: LST 1515 rationalise cost centre codes in tests (#384)
*
</commit_message>
<xml_diff>
--- a/forecast/test/test_assets/upload_test.xlsx
+++ b/forecast/test/test_assets/upload_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stronal/PycharmProjects/fido/forecast/test/test_assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stronal/PycharmProjects/fft/forecast/test/test_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A4CD60-428F-7648-8ABB-3E208882A10D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3B4261-AD5D-9B44-B6AE-8BA85681AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15820" xr2:uid="{9054BADA-7C02-1543-A56F-A27503B8E715}"/>
+    <workbookView xWindow="-27740" yWindow="-5000" windowWidth="27040" windowHeight="15260" xr2:uid="{9054BADA-7C02-1543-A56F-A27503B8E715}"/>
   </bookViews>
   <sheets>
     <sheet name="FNDWRR" sheetId="1" r:id="rId1"/>
@@ -42,16 +42,16 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>3000-30000-109189-18162001-310530-00000-00000-0000-0000-0000</t>
+    <t>3000-30000-888812-18162001-310530-00000-00000-0000-0000-0000</t>
   </si>
   <si>
-    <t>3000-30000-109189-52191003-310530-00000-00000-0000-0000-0000</t>
+    <t>3000-30000-888812-18162001-310540-00000-00000-0000-0000-0000</t>
   </si>
   <si>
-    <t>3000-30000-109189-18162001-310540-00000-00000-0000-0000-0000</t>
+    <t>3000-30000-888812-52191003-310530-00000-00000-0000-0000-0000</t>
   </si>
   <si>
-    <t>3000-30000-109189-52191003-310540-00000-00000-0000-0000-0000</t>
+    <t>3000-30000-888812-52191003-310540-00000-00000-0000-0000-0000</t>
   </si>
 </sst>
 </file>
@@ -341,40 +341,40 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -693,7 +693,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,13 +722,13 @@
       <c r="D2" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="10.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="10.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -739,27 +739,27 @@
       <c r="C6" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:7" ht="10.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="1:7" ht="11" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -783,7 +783,7 @@
       <c r="B14" s="24"/>
       <c r="C14" s="25"/>
       <c r="D14" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="18">
@@ -796,7 +796,7 @@
       <c r="B15" s="24"/>
       <c r="C15" s="25"/>
       <c r="D15" s="16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="18">
@@ -866,13 +866,13 @@
       <c r="E22" s="22"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
@@ -881,6 +881,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
@@ -892,11 +897,6 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>